<commit_message>
#Feature: Added patient_prep_test table schema #Feature: PREP functionality when Adding Patient #Feature: Integrated Download and Import for Order Module(v2) #Fix:Use of REPLACE instead of INSERT for sync schemas #Fix: D-MAPS(v2) template missing expected and actual fields
</commit_message>
<xml_diff>
--- a/assets/templates/orders/v2/cdrr_aggregate.xlsx
+++ b/assets/templates/orders/v2/cdrr_aggregate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marete\Downloads\Compressed\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ADT\assets\templates\orders\v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1539,9 +1539,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1952,6 +1949,63 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1976,67 +2030,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2357,27 +2357,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="134.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="90" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" style="90" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" style="90" customWidth="1"/>
-    <col min="6" max="6" width="51.6640625" style="90" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="90" customWidth="1"/>
-    <col min="8" max="8" width="29.44140625" style="90" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" style="90" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" style="90" customWidth="1"/>
-    <col min="11" max="11" width="2.6640625" style="90" customWidth="1"/>
-    <col min="12" max="12" width="39" style="90" customWidth="1"/>
-    <col min="13" max="13" width="38.6640625" style="90" customWidth="1"/>
-    <col min="14" max="14" width="2.6640625" style="90" customWidth="1"/>
-    <col min="15" max="15" width="27.6640625" style="90" customWidth="1"/>
+    <col min="3" max="3" width="26" style="89" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" style="89" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" style="89" customWidth="1"/>
+    <col min="6" max="6" width="51.6640625" style="89" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="89" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" style="89" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" style="89" customWidth="1"/>
+    <col min="10" max="10" width="35.6640625" style="89" customWidth="1"/>
+    <col min="11" max="11" width="2.6640625" style="89" customWidth="1"/>
+    <col min="12" max="12" width="39" style="89" customWidth="1"/>
+    <col min="13" max="13" width="38.6640625" style="89" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" style="89" customWidth="1"/>
+    <col min="15" max="15" width="27.6640625" style="89" customWidth="1"/>
     <col min="16" max="16" width="27.109375" style="3" customWidth="1"/>
     <col min="17" max="17" width="25.44140625" style="3" customWidth="1"/>
     <col min="18" max="18" width="35.6640625" style="3" customWidth="1"/>
@@ -2408,2338 +2408,2331 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="2:21" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="B2" s="183" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="6" t="s">
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="183"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="183"/>
+      <c r="M2" s="183"/>
+      <c r="N2" s="183"/>
+      <c r="O2" s="183"/>
+      <c r="P2" s="183"/>
+      <c r="Q2" s="183"/>
+      <c r="R2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:21" s="12" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="2:21" s="11" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-    </row>
-    <row r="5" spans="2:21" s="12" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="K4" s="10"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="2:21" s="11" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-    </row>
-    <row r="6" spans="2:21" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-    </row>
-    <row r="7" spans="2:21" s="12" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+      <c r="K5" s="10"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+    </row>
+    <row r="6" spans="2:21" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="2:21" s="11" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="7" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="2:21" s="12" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="K7" s="13"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="2:21" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="16" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="16" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-    </row>
-    <row r="9" spans="2:21" s="12" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="17"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-    </row>
-    <row r="10" spans="2:21" s="12" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="17"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="155" t="s">
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="2:21" s="11" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="16"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+    </row>
+    <row r="10" spans="2:21" s="11" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="16"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="156"/>
-      <c r="F10" s="156"/>
-      <c r="G10" s="156"/>
-      <c r="H10" s="156"/>
-      <c r="I10" s="156"/>
-      <c r="J10" s="157"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="158" t="s">
+      <c r="E10" s="174"/>
+      <c r="F10" s="174"/>
+      <c r="G10" s="174"/>
+      <c r="H10" s="174"/>
+      <c r="I10" s="174"/>
+      <c r="J10" s="175"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="159"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="155" t="s">
+      <c r="M10" s="177"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="P10" s="156"/>
-      <c r="Q10" s="156"/>
-      <c r="R10" s="157"/>
+      <c r="P10" s="174"/>
+      <c r="Q10" s="174"/>
+      <c r="R10" s="175"/>
     </row>
     <row r="11" spans="2:21" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="160" t="s">
+      <c r="D11" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="160" t="s">
+      <c r="E11" s="178" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="160" t="s">
+      <c r="F11" s="178" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="160" t="s">
+      <c r="G11" s="178" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="162" t="s">
+      <c r="H11" s="180" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="163"/>
-      <c r="J11" s="164" t="s">
+      <c r="I11" s="162"/>
+      <c r="J11" s="163" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="166" t="s">
+      <c r="K11" s="20"/>
+      <c r="L11" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="173" t="s">
+      <c r="M11" s="159" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="175" t="s">
+      <c r="N11" s="21"/>
+      <c r="O11" s="161" t="s">
         <v>25</v>
       </c>
-      <c r="P11" s="163"/>
-      <c r="Q11" s="164" t="s">
+      <c r="P11" s="162"/>
+      <c r="Q11" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="R11" s="176" t="s">
+      <c r="R11" s="165" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:21" s="31" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="161"/>
-      <c r="E12" s="161"/>
-      <c r="F12" s="161"/>
-      <c r="G12" s="161"/>
-      <c r="H12" s="25" t="s">
+    <row r="12" spans="2:21" s="30" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="179"/>
+      <c r="E12" s="179"/>
+      <c r="F12" s="179"/>
+      <c r="G12" s="179"/>
+      <c r="H12" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="165"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="167"/>
-      <c r="M12" s="174"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="28" t="s">
+      <c r="J12" s="164"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="182"/>
+      <c r="M12" s="160"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="29" t="s">
+      <c r="P12" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="Q12" s="165"/>
-      <c r="R12" s="177"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
+      <c r="Q12" s="164"/>
+      <c r="R12" s="166"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
     </row>
     <row r="13" spans="2:21" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="37" t="s">
+      <c r="I13" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="38"/>
-      <c r="L13" s="34" t="s">
+      <c r="K13" s="37"/>
+      <c r="L13" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="34" t="s">
+      <c r="M13" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="39"/>
-      <c r="O13" s="40" t="s">
+      <c r="N13" s="38"/>
+      <c r="O13" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="P13" s="41" t="s">
+      <c r="P13" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="Q13" s="42" t="s">
+      <c r="Q13" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="R13" s="43" t="s">
+      <c r="R13" s="42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:21" s="12" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="178" t="s">
+    <row r="14" spans="2:21" s="11" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="167" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="179"/>
-      <c r="F14" s="179"/>
-      <c r="G14" s="179"/>
-      <c r="H14" s="179"/>
-      <c r="I14" s="179"/>
-      <c r="J14" s="179"/>
-      <c r="K14" s="179"/>
-      <c r="L14" s="179"/>
-      <c r="M14" s="179"/>
-      <c r="N14" s="179"/>
-      <c r="O14" s="179"/>
-      <c r="P14" s="179"/>
-      <c r="Q14" s="179"/>
-      <c r="R14" s="180"/>
-    </row>
-    <row r="15" spans="2:21" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="181" t="s">
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="168"/>
+      <c r="F14" s="168"/>
+      <c r="G14" s="168"/>
+      <c r="H14" s="168"/>
+      <c r="I14" s="168"/>
+      <c r="J14" s="168"/>
+      <c r="K14" s="168"/>
+      <c r="L14" s="168"/>
+      <c r="M14" s="168"/>
+      <c r="N14" s="168"/>
+      <c r="O14" s="168"/>
+      <c r="P14" s="168"/>
+      <c r="Q14" s="168"/>
+      <c r="R14" s="169"/>
+    </row>
+    <row r="15" spans="2:21" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="182"/>
-      <c r="D15" s="182"/>
-      <c r="E15" s="182"/>
-      <c r="F15" s="182"/>
-      <c r="G15" s="182"/>
-      <c r="H15" s="182"/>
-      <c r="I15" s="182"/>
-      <c r="J15" s="182"/>
-      <c r="K15" s="182"/>
-      <c r="L15" s="182"/>
-      <c r="M15" s="182"/>
-      <c r="N15" s="182"/>
-      <c r="O15" s="182"/>
-      <c r="P15" s="182"/>
-      <c r="Q15" s="182"/>
-      <c r="R15" s="183"/>
-      <c r="S15" s="9"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="171"/>
+      <c r="F15" s="171"/>
+      <c r="G15" s="171"/>
+      <c r="H15" s="171"/>
+      <c r="I15" s="171"/>
+      <c r="J15" s="171"/>
+      <c r="K15" s="171"/>
+      <c r="L15" s="171"/>
+      <c r="M15" s="171"/>
+      <c r="N15" s="171"/>
+      <c r="O15" s="171"/>
+      <c r="P15" s="171"/>
+      <c r="Q15" s="171"/>
+      <c r="R15" s="172"/>
+      <c r="S15" s="8"/>
     </row>
     <row r="16" spans="2:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="151" t="s">
+      <c r="B16" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="43">
         <v>30</v>
       </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="52"/>
-      <c r="P16" s="53"/>
-      <c r="Q16" s="54"/>
-      <c r="R16" s="55">
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="54">
         <f>(L16*3)-J16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="151" t="s">
+      <c r="B17" s="150" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="43">
         <v>30</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="52"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="55">
+      <c r="D17" s="44"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="54">
         <f t="shared" ref="R17:R72" si="0">(L17*3)-J17</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:18" s="3" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="151" t="s">
+      <c r="B18" s="150" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="43">
         <v>30</v>
       </c>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="60"/>
-      <c r="R18" s="55">
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:18" s="3" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="150" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="43">
         <v>30</v>
       </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="52"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="54"/>
-      <c r="R19" s="55">
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="53"/>
+      <c r="R19" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:18" s="3" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="151" t="s">
+      <c r="B20" s="150" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="43">
         <v>60</v>
       </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="52"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="55">
+      <c r="D20" s="44"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="52"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:18" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="151" t="s">
+      <c r="B21" s="150" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="44">
+      <c r="C21" s="43">
         <v>30</v>
       </c>
-      <c r="D21" s="45"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="52"/>
-      <c r="P21" s="53"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="55">
+      <c r="D21" s="44"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="53"/>
+      <c r="R21" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:18" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="151" t="s">
+      <c r="B22" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="44">
+      <c r="C22" s="43">
         <v>60</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="64"/>
-      <c r="P22" s="53"/>
-      <c r="Q22" s="65"/>
-      <c r="R22" s="55">
+      <c r="D22" s="60"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="64"/>
+      <c r="R22" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="151" t="s">
+      <c r="B23" s="150" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="44">
+      <c r="C23" s="43">
         <v>60</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="64"/>
-      <c r="P23" s="53"/>
-      <c r="Q23" s="65"/>
-      <c r="R23" s="55">
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="52"/>
+      <c r="Q23" s="64"/>
+      <c r="R23" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:18" s="3" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="151" t="s">
+      <c r="B24" s="150" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="44">
+      <c r="C24" s="43">
         <v>30</v>
       </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="55">
+      <c r="D24" s="44"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:18" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="151" t="s">
+      <c r="B25" s="150" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="44">
+      <c r="C25" s="43">
         <v>30</v>
       </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="52"/>
-      <c r="P25" s="53"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="55">
+      <c r="D25" s="44"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="52"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:18" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="151" t="s">
+      <c r="B26" s="150" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="44">
+      <c r="C26" s="43">
         <v>30</v>
       </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="50"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="52"/>
-      <c r="P26" s="53"/>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="55">
+      <c r="D26" s="44"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="52"/>
+      <c r="Q26" s="53"/>
+      <c r="R26" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="151" t="s">
+      <c r="B27" s="150" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="44">
+      <c r="C27" s="43">
         <v>60</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="64"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="65"/>
-      <c r="R27" s="55">
+      <c r="D27" s="60"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="64"/>
+      <c r="R27" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="151" t="s">
+      <c r="B28" s="150" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="44">
+      <c r="C28" s="43">
         <v>120</v>
       </c>
-      <c r="D28" s="61"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="63"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="64"/>
-      <c r="P28" s="53"/>
-      <c r="Q28" s="65"/>
-      <c r="R28" s="55">
+      <c r="D28" s="60"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="64"/>
+      <c r="R28" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="151" t="s">
+      <c r="B29" s="150" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="44">
+      <c r="C29" s="43">
         <v>60</v>
       </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="52"/>
-      <c r="P29" s="53"/>
-      <c r="Q29" s="54"/>
-      <c r="R29" s="55">
+      <c r="D29" s="44"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="151" t="s">
+      <c r="B30" s="150" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="44">
+      <c r="C30" s="43">
         <v>30</v>
       </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="66"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="67"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="68">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" s="12" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="152" t="s">
+      <c r="D30" s="44"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="65"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="151" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="44">
+      <c r="C31" s="43">
         <v>60</v>
       </c>
-      <c r="D31" s="69"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
-      <c r="N31" s="71"/>
-      <c r="O31" s="72"/>
-      <c r="P31" s="72"/>
-      <c r="Q31" s="72"/>
-      <c r="R31" s="68">
+      <c r="D31" s="68"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="70"/>
+      <c r="O31" s="71"/>
+      <c r="P31" s="71"/>
+      <c r="Q31" s="71"/>
+      <c r="R31" s="67">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="151" t="s">
+      <c r="B32" s="150" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="44">
+      <c r="C32" s="43">
         <v>60</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="52"/>
-      <c r="P32" s="53"/>
-      <c r="Q32" s="54"/>
-      <c r="R32" s="55">
+      <c r="D32" s="44"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="51"/>
+      <c r="P32" s="52"/>
+      <c r="Q32" s="53"/>
+      <c r="R32" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:22" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="151" t="s">
+      <c r="B33" s="150" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="44">
+      <c r="C33" s="43">
         <v>60</v>
       </c>
-      <c r="D33" s="45"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="52"/>
-      <c r="P33" s="53"/>
-      <c r="Q33" s="54"/>
-      <c r="R33" s="55">
+      <c r="D33" s="44"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="52"/>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:22" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="151" t="s">
+      <c r="B34" s="150" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="44">
+      <c r="C34" s="43">
         <v>60</v>
       </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="53"/>
-      <c r="Q34" s="54"/>
-      <c r="R34" s="55">
+      <c r="D34" s="44"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="51"/>
+      <c r="P34" s="52"/>
+      <c r="Q34" s="53"/>
+      <c r="R34" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:22" s="3" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="151" t="s">
+      <c r="B35" s="150" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="44">
+      <c r="C35" s="43">
         <v>30</v>
       </c>
-      <c r="D35" s="45"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="53"/>
-      <c r="Q35" s="54"/>
-      <c r="R35" s="55">
+      <c r="D35" s="44"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="51"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="53"/>
+      <c r="R35" s="54">
         <f>(L35*3)-J35</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:22" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="73" t="s">
+      <c r="B36" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="73"/>
-      <c r="I36" s="73"/>
-      <c r="J36" s="73"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
-      <c r="M36" s="73"/>
-      <c r="N36" s="73"/>
-      <c r="O36" s="73"/>
-      <c r="P36" s="73"/>
-      <c r="Q36" s="73"/>
-      <c r="R36" s="74"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
+      <c r="M36" s="72"/>
+      <c r="N36" s="72"/>
+      <c r="O36" s="72"/>
+      <c r="P36" s="72"/>
+      <c r="Q36" s="72"/>
+      <c r="R36" s="73"/>
       <c r="U36" s="4"/>
     </row>
     <row r="37" spans="2:22" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="151" t="s">
+      <c r="B37" s="150" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="44">
+      <c r="C37" s="43">
         <v>60</v>
       </c>
-      <c r="D37" s="45"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="51"/>
-      <c r="O37" s="52"/>
-      <c r="P37" s="53"/>
-      <c r="Q37" s="54"/>
-      <c r="R37" s="55">
+      <c r="D37" s="44"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="47"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="52"/>
+      <c r="Q37" s="53"/>
+      <c r="R37" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:22" ht="54" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="151" t="s">
+      <c r="B38" s="150" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="44">
+      <c r="C38" s="43">
         <v>60</v>
       </c>
-      <c r="D38" s="45"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="50"/>
-      <c r="N38" s="51"/>
-      <c r="O38" s="52"/>
-      <c r="P38" s="53"/>
-      <c r="Q38" s="54"/>
-      <c r="R38" s="55">
+      <c r="D38" s="44"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="48"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="52"/>
+      <c r="Q38" s="53"/>
+      <c r="R38" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:22" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="151" t="s">
+      <c r="B39" s="150" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="44">
+      <c r="C39" s="43">
         <v>60</v>
       </c>
-      <c r="D39" s="45"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="50"/>
-      <c r="N39" s="51"/>
-      <c r="O39" s="52"/>
-      <c r="P39" s="53"/>
-      <c r="Q39" s="54"/>
-      <c r="R39" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T39" s="75"/>
-      <c r="U39" s="76"/>
-      <c r="V39" s="77"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="52"/>
+      <c r="Q39" s="53"/>
+      <c r="R39" s="54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="74"/>
+      <c r="U39" s="75"/>
+      <c r="V39" s="76"/>
     </row>
     <row r="40" spans="2:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="151" t="s">
+      <c r="B40" s="150" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="44">
+      <c r="C40" s="43">
         <v>60</v>
       </c>
-      <c r="D40" s="45"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="50"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="52"/>
-      <c r="P40" s="53"/>
-      <c r="Q40" s="54"/>
-      <c r="R40" s="55">
+      <c r="D40" s="44"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="48"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="51"/>
+      <c r="P40" s="52"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="151" t="s">
+      <c r="B41" s="150" t="s">
         <v>115</v>
       </c>
-      <c r="C41" s="44">
+      <c r="C41" s="43">
         <v>90</v>
       </c>
-      <c r="D41" s="45"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="50"/>
-      <c r="N41" s="51"/>
-      <c r="O41" s="52"/>
-      <c r="P41" s="53"/>
-      <c r="Q41" s="54"/>
-      <c r="R41" s="55">
+      <c r="D41" s="44"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="51"/>
+      <c r="P41" s="52"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="153" t="s">
+      <c r="B42" s="152" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="78" t="s">
+      <c r="C42" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="45"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="47"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="50"/>
-      <c r="N42" s="51"/>
-      <c r="O42" s="52"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="55">
+      <c r="D42" s="44"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="48"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="51"/>
+      <c r="P42" s="52"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="153" t="s">
+      <c r="B43" s="152" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="78" t="s">
+      <c r="C43" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="45"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="46"/>
-      <c r="I43" s="46"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="51"/>
-      <c r="O43" s="52"/>
-      <c r="P43" s="53"/>
-      <c r="Q43" s="54"/>
-      <c r="R43" s="55">
+      <c r="D43" s="44"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="51"/>
+      <c r="P43" s="52"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="151" t="s">
+      <c r="B44" s="150" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="78">
+      <c r="C44" s="77">
         <v>120</v>
       </c>
-      <c r="D44" s="45"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="51"/>
-      <c r="O44" s="52"/>
-      <c r="P44" s="53"/>
-      <c r="Q44" s="54"/>
-      <c r="R44" s="55">
+      <c r="D44" s="44"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="51"/>
+      <c r="P44" s="52"/>
+      <c r="Q44" s="53"/>
+      <c r="R44" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:22" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="151" t="s">
+      <c r="B45" s="150" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="78" t="s">
+      <c r="C45" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="45"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="49"/>
-      <c r="M45" s="50"/>
-      <c r="N45" s="51"/>
-      <c r="O45" s="52"/>
-      <c r="P45" s="53"/>
-      <c r="Q45" s="54"/>
-      <c r="R45" s="55">
+      <c r="D45" s="44"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="51"/>
+      <c r="P45" s="52"/>
+      <c r="Q45" s="53"/>
+      <c r="R45" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:22" s="3" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="151" t="s">
+      <c r="B46" s="150" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="78" t="s">
+      <c r="C46" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="45"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="49"/>
-      <c r="M46" s="50"/>
-      <c r="N46" s="51"/>
-      <c r="O46" s="52"/>
-      <c r="P46" s="53"/>
-      <c r="Q46" s="54"/>
-      <c r="R46" s="55">
+      <c r="D46" s="44"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="49"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="51"/>
+      <c r="P46" s="52"/>
+      <c r="Q46" s="53"/>
+      <c r="R46" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:22" s="3" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="151" t="s">
+      <c r="B47" s="150" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="78">
+      <c r="C47" s="77">
         <v>60</v>
       </c>
-      <c r="D47" s="45"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="46"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="49"/>
-      <c r="M47" s="50"/>
-      <c r="N47" s="51"/>
-      <c r="O47" s="52"/>
-      <c r="P47" s="53"/>
-      <c r="Q47" s="54"/>
-      <c r="R47" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:22" s="12" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="152" t="s">
+      <c r="D47" s="44"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="45"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="52"/>
+      <c r="Q47" s="53"/>
+      <c r="R47" s="54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:22" s="11" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="151" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="79">
+      <c r="C48" s="78">
         <v>240</v>
       </c>
-      <c r="D48" s="45"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="46"/>
-      <c r="I48" s="46"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="49"/>
-      <c r="M48" s="50"/>
-      <c r="N48" s="51"/>
-      <c r="O48" s="52"/>
-      <c r="P48" s="53"/>
-      <c r="Q48" s="54"/>
-      <c r="R48" s="55">
+      <c r="D48" s="44"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="50"/>
+      <c r="O48" s="51"/>
+      <c r="P48" s="52"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:18" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="151" t="s">
+      <c r="B49" s="150" t="s">
         <v>121</v>
       </c>
-      <c r="C49" s="79">
+      <c r="C49" s="78">
         <v>480</v>
       </c>
-      <c r="D49" s="45"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="46"/>
-      <c r="I49" s="46"/>
-      <c r="J49" s="47"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="49"/>
-      <c r="M49" s="50"/>
-      <c r="N49" s="51"/>
-      <c r="O49" s="52"/>
-      <c r="P49" s="53"/>
-      <c r="Q49" s="54"/>
-      <c r="R49" s="55">
+      <c r="D49" s="44"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="49"/>
+      <c r="N49" s="50"/>
+      <c r="O49" s="51"/>
+      <c r="P49" s="52"/>
+      <c r="Q49" s="53"/>
+      <c r="R49" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:18" s="3" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="151" t="s">
+      <c r="B50" s="150" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="78" t="s">
+      <c r="C50" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="D50" s="45"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="47"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="50"/>
-      <c r="N50" s="51"/>
-      <c r="O50" s="52"/>
-      <c r="P50" s="53"/>
-      <c r="Q50" s="54"/>
-      <c r="R50" s="55">
+      <c r="D50" s="44"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="49"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="51"/>
+      <c r="P50" s="52"/>
+      <c r="Q50" s="53"/>
+      <c r="R50" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:18" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="151" t="s">
+      <c r="B51" s="150" t="s">
         <v>123</v>
       </c>
-      <c r="C51" s="78">
+      <c r="C51" s="77">
         <v>60</v>
       </c>
-      <c r="D51" s="45"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="46"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="46"/>
-      <c r="I51" s="46"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="49"/>
-      <c r="M51" s="50"/>
-      <c r="N51" s="51"/>
-      <c r="O51" s="52"/>
-      <c r="P51" s="53"/>
-      <c r="Q51" s="54"/>
-      <c r="R51" s="55">
+      <c r="D51" s="44"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="49"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="51"/>
+      <c r="P51" s="52"/>
+      <c r="Q51" s="53"/>
+      <c r="R51" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:18" s="3" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="151" t="s">
+      <c r="B52" s="150" t="s">
         <v>124</v>
       </c>
-      <c r="C52" s="78">
+      <c r="C52" s="77">
         <v>60</v>
       </c>
-      <c r="D52" s="45"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="45"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="47"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="49"/>
-      <c r="M52" s="50"/>
-      <c r="N52" s="51"/>
-      <c r="O52" s="52"/>
-      <c r="P52" s="53"/>
-      <c r="Q52" s="54"/>
-      <c r="R52" s="55">
+      <c r="D52" s="44"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="46"/>
+      <c r="K52" s="47"/>
+      <c r="L52" s="48"/>
+      <c r="M52" s="49"/>
+      <c r="N52" s="50"/>
+      <c r="O52" s="51"/>
+      <c r="P52" s="52"/>
+      <c r="Q52" s="53"/>
+      <c r="R52" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="151" t="s">
+      <c r="B53" s="150" t="s">
         <v>125</v>
       </c>
-      <c r="C53" s="78">
+      <c r="C53" s="77">
         <v>60</v>
       </c>
-      <c r="D53" s="45"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="46"/>
-      <c r="G53" s="45"/>
-      <c r="H53" s="46"/>
-      <c r="I53" s="46"/>
-      <c r="J53" s="47"/>
-      <c r="K53" s="48"/>
-      <c r="L53" s="49"/>
-      <c r="M53" s="50"/>
-      <c r="N53" s="51"/>
-      <c r="O53" s="52"/>
-      <c r="P53" s="53"/>
-      <c r="Q53" s="54"/>
-      <c r="R53" s="55">
+      <c r="D53" s="44"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="47"/>
+      <c r="L53" s="48"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="50"/>
+      <c r="O53" s="51"/>
+      <c r="P53" s="52"/>
+      <c r="Q53" s="53"/>
+      <c r="R53" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="151" t="s">
+      <c r="B54" s="150" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="78">
+      <c r="C54" s="77">
         <v>60</v>
       </c>
-      <c r="D54" s="45"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="46"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="47"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="49"/>
-      <c r="M54" s="50"/>
-      <c r="N54" s="51"/>
-      <c r="O54" s="52"/>
-      <c r="P54" s="53"/>
-      <c r="Q54" s="54"/>
-      <c r="R54" s="55">
+      <c r="D54" s="44"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="44"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="47"/>
+      <c r="L54" s="48"/>
+      <c r="M54" s="49"/>
+      <c r="N54" s="50"/>
+      <c r="O54" s="51"/>
+      <c r="P54" s="52"/>
+      <c r="Q54" s="53"/>
+      <c r="R54" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:18" s="3" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B55" s="151" t="s">
+      <c r="B55" s="150" t="s">
         <v>127</v>
       </c>
-      <c r="C55" s="78" t="s">
+      <c r="C55" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="45"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="46"/>
-      <c r="I55" s="46"/>
-      <c r="J55" s="47"/>
-      <c r="K55" s="48"/>
-      <c r="L55" s="49"/>
-      <c r="M55" s="50"/>
-      <c r="N55" s="51"/>
-      <c r="O55" s="52"/>
-      <c r="P55" s="53"/>
-      <c r="Q55" s="54"/>
-      <c r="R55" s="55">
+      <c r="D55" s="44"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="44"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="47"/>
+      <c r="L55" s="48"/>
+      <c r="M55" s="49"/>
+      <c r="N55" s="50"/>
+      <c r="O55" s="51"/>
+      <c r="P55" s="52"/>
+      <c r="Q55" s="53"/>
+      <c r="R55" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="80" t="s">
+      <c r="B56" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="80"/>
-      <c r="D56" s="80"/>
-      <c r="E56" s="80"/>
-      <c r="F56" s="80"/>
-      <c r="G56" s="80"/>
-      <c r="H56" s="80"/>
-      <c r="I56" s="80"/>
-      <c r="J56" s="80"/>
-      <c r="K56" s="80"/>
-      <c r="L56" s="80"/>
-      <c r="M56" s="80"/>
-      <c r="N56" s="80"/>
-      <c r="O56" s="80"/>
-      <c r="P56" s="80"/>
-      <c r="Q56" s="80"/>
-      <c r="R56" s="81"/>
+      <c r="C56" s="79"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="79"/>
+      <c r="G56" s="79"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="79"/>
+      <c r="J56" s="79"/>
+      <c r="K56" s="79"/>
+      <c r="L56" s="79"/>
+      <c r="M56" s="79"/>
+      <c r="N56" s="79"/>
+      <c r="O56" s="79"/>
+      <c r="P56" s="79"/>
+      <c r="Q56" s="79"/>
+      <c r="R56" s="80"/>
     </row>
     <row r="57" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="151" t="s">
+      <c r="B57" s="150" t="s">
         <v>128</v>
       </c>
-      <c r="C57" s="44">
+      <c r="C57" s="43">
         <v>100</v>
       </c>
-      <c r="D57" s="45"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="46"/>
-      <c r="I57" s="46"/>
-      <c r="J57" s="47"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="49"/>
-      <c r="M57" s="50"/>
-      <c r="N57" s="51"/>
-      <c r="O57" s="52"/>
-      <c r="P57" s="53"/>
-      <c r="Q57" s="54"/>
-      <c r="R57" s="55">
+      <c r="D57" s="44"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="46"/>
+      <c r="K57" s="47"/>
+      <c r="L57" s="48"/>
+      <c r="M57" s="49"/>
+      <c r="N57" s="50"/>
+      <c r="O57" s="51"/>
+      <c r="P57" s="52"/>
+      <c r="Q57" s="53"/>
+      <c r="R57" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:18" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="151" t="s">
+      <c r="B58" s="150" t="s">
         <v>129</v>
       </c>
-      <c r="C58" s="82" t="s">
+      <c r="C58" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="D58" s="45"/>
-      <c r="E58" s="46"/>
-      <c r="F58" s="46"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="46"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="47"/>
-      <c r="K58" s="48"/>
-      <c r="L58" s="49"/>
-      <c r="M58" s="50"/>
-      <c r="N58" s="51"/>
-      <c r="O58" s="52"/>
-      <c r="P58" s="53"/>
-      <c r="Q58" s="54"/>
-      <c r="R58" s="55">
+      <c r="D58" s="44"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="48"/>
+      <c r="M58" s="49"/>
+      <c r="N58" s="50"/>
+      <c r="O58" s="51"/>
+      <c r="P58" s="52"/>
+      <c r="Q58" s="53"/>
+      <c r="R58" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:18" ht="55.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="151" t="s">
+      <c r="B59" s="150" t="s">
         <v>130</v>
       </c>
-      <c r="C59" s="44">
+      <c r="C59" s="43">
         <v>100</v>
       </c>
-      <c r="D59" s="45"/>
-      <c r="E59" s="46"/>
-      <c r="F59" s="46"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="46"/>
-      <c r="I59" s="46"/>
-      <c r="J59" s="47"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="50"/>
-      <c r="N59" s="51"/>
-      <c r="O59" s="52"/>
-      <c r="P59" s="53"/>
-      <c r="Q59" s="54"/>
-      <c r="R59" s="55">
+      <c r="D59" s="44"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="47"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="49"/>
+      <c r="N59" s="50"/>
+      <c r="O59" s="51"/>
+      <c r="P59" s="52"/>
+      <c r="Q59" s="53"/>
+      <c r="R59" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="151" t="s">
+      <c r="B60" s="150" t="s">
         <v>131</v>
       </c>
-      <c r="C60" s="83">
+      <c r="C60" s="82">
         <v>100</v>
       </c>
-      <c r="D60" s="45"/>
-      <c r="E60" s="46"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="46"/>
-      <c r="I60" s="46"/>
-      <c r="J60" s="47"/>
-      <c r="K60" s="48"/>
-      <c r="L60" s="49"/>
-      <c r="M60" s="50"/>
-      <c r="N60" s="51"/>
-      <c r="O60" s="52"/>
-      <c r="P60" s="53"/>
-      <c r="Q60" s="54"/>
-      <c r="R60" s="55">
+      <c r="D60" s="44"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="45"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="47"/>
+      <c r="L60" s="48"/>
+      <c r="M60" s="49"/>
+      <c r="N60" s="50"/>
+      <c r="O60" s="51"/>
+      <c r="P60" s="52"/>
+      <c r="Q60" s="53"/>
+      <c r="R60" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="151" t="s">
+      <c r="B61" s="150" t="s">
         <v>132</v>
       </c>
-      <c r="C61" s="83">
+      <c r="C61" s="82">
         <v>100</v>
       </c>
-      <c r="D61" s="46"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="46"/>
-      <c r="H61" s="46"/>
-      <c r="I61" s="46"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="84"/>
-      <c r="L61" s="46"/>
-      <c r="M61" s="46"/>
-      <c r="N61" s="84"/>
-      <c r="O61" s="46"/>
-      <c r="P61" s="67"/>
-      <c r="Q61" s="46"/>
-      <c r="R61" s="55">
+      <c r="D61" s="45"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="45"/>
+      <c r="J61" s="45"/>
+      <c r="K61" s="83"/>
+      <c r="L61" s="45"/>
+      <c r="M61" s="45"/>
+      <c r="N61" s="83"/>
+      <c r="O61" s="45"/>
+      <c r="P61" s="66"/>
+      <c r="Q61" s="45"/>
+      <c r="R61" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B62" s="151" t="s">
+      <c r="B62" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="85" t="s">
+      <c r="C62" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="D62" s="46"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="46"/>
-      <c r="H62" s="46"/>
-      <c r="I62" s="46"/>
-      <c r="J62" s="46"/>
-      <c r="K62" s="84"/>
-      <c r="L62" s="46"/>
-      <c r="M62" s="46"/>
-      <c r="N62" s="84"/>
-      <c r="O62" s="46"/>
-      <c r="P62" s="67"/>
-      <c r="Q62" s="46"/>
-      <c r="R62" s="55">
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="83"/>
+      <c r="L62" s="45"/>
+      <c r="M62" s="45"/>
+      <c r="N62" s="83"/>
+      <c r="O62" s="45"/>
+      <c r="P62" s="66"/>
+      <c r="Q62" s="45"/>
+      <c r="R62" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B63" s="151" t="s">
+      <c r="B63" s="150" t="s">
         <v>133</v>
       </c>
-      <c r="C63" s="44">
+      <c r="C63" s="43">
         <v>30</v>
       </c>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
-      <c r="H63" s="46"/>
-      <c r="I63" s="46"/>
-      <c r="J63" s="46"/>
-      <c r="K63" s="84"/>
-      <c r="L63" s="46"/>
-      <c r="M63" s="46"/>
-      <c r="N63" s="84"/>
-      <c r="O63" s="46"/>
-      <c r="P63" s="67"/>
-      <c r="Q63" s="46"/>
-      <c r="R63" s="55">
+      <c r="D63" s="45"/>
+      <c r="E63" s="45"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="45"/>
+      <c r="J63" s="45"/>
+      <c r="K63" s="83"/>
+      <c r="L63" s="45"/>
+      <c r="M63" s="45"/>
+      <c r="N63" s="83"/>
+      <c r="O63" s="45"/>
+      <c r="P63" s="66"/>
+      <c r="Q63" s="45"/>
+      <c r="R63" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B64" s="151" t="s">
+      <c r="B64" s="150" t="s">
         <v>59</v>
       </c>
-      <c r="C64" s="44">
+      <c r="C64" s="43">
         <v>100</v>
       </c>
-      <c r="D64" s="46"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="46"/>
-      <c r="G64" s="46"/>
-      <c r="H64" s="46"/>
-      <c r="I64" s="46"/>
-      <c r="J64" s="46"/>
-      <c r="K64" s="84"/>
-      <c r="L64" s="46"/>
-      <c r="M64" s="46"/>
-      <c r="N64" s="84"/>
-      <c r="O64" s="46"/>
-      <c r="P64" s="67"/>
-      <c r="Q64" s="46"/>
-      <c r="R64" s="55">
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="45"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="83"/>
+      <c r="L64" s="45"/>
+      <c r="M64" s="45"/>
+      <c r="N64" s="83"/>
+      <c r="O64" s="45"/>
+      <c r="P64" s="66"/>
+      <c r="Q64" s="45"/>
+      <c r="R64" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B65" s="151" t="s">
+      <c r="B65" s="150" t="s">
         <v>134</v>
       </c>
-      <c r="C65" s="44">
+      <c r="C65" s="43">
         <v>100</v>
       </c>
-      <c r="D65" s="46"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="46"/>
-      <c r="G65" s="46"/>
-      <c r="H65" s="46"/>
-      <c r="I65" s="46"/>
-      <c r="J65" s="46"/>
-      <c r="K65" s="84"/>
-      <c r="L65" s="46"/>
-      <c r="M65" s="46"/>
-      <c r="N65" s="84"/>
-      <c r="O65" s="46"/>
-      <c r="P65" s="67"/>
-      <c r="Q65" s="46"/>
-      <c r="R65" s="55">
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="45"/>
+      <c r="I65" s="45"/>
+      <c r="J65" s="45"/>
+      <c r="K65" s="83"/>
+      <c r="L65" s="45"/>
+      <c r="M65" s="45"/>
+      <c r="N65" s="83"/>
+      <c r="O65" s="45"/>
+      <c r="P65" s="66"/>
+      <c r="Q65" s="45"/>
+      <c r="R65" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B66" s="151" t="s">
+      <c r="B66" s="150" t="s">
         <v>135</v>
       </c>
-      <c r="C66" s="83">
+      <c r="C66" s="82">
         <v>100</v>
       </c>
-      <c r="D66" s="46"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="46"/>
-      <c r="H66" s="46"/>
-      <c r="I66" s="46"/>
-      <c r="J66" s="46"/>
-      <c r="K66" s="84"/>
-      <c r="L66" s="46"/>
-      <c r="M66" s="46"/>
-      <c r="N66" s="84"/>
-      <c r="O66" s="46"/>
-      <c r="P66" s="67"/>
-      <c r="Q66" s="46"/>
-      <c r="R66" s="55">
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="45"/>
+      <c r="J66" s="45"/>
+      <c r="K66" s="83"/>
+      <c r="L66" s="45"/>
+      <c r="M66" s="45"/>
+      <c r="N66" s="83"/>
+      <c r="O66" s="45"/>
+      <c r="P66" s="66"/>
+      <c r="Q66" s="45"/>
+      <c r="R66" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="154" t="s">
+      <c r="B67" s="153" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="86">
+      <c r="C67" s="85">
         <v>100</v>
       </c>
-      <c r="D67" s="83"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="46"/>
-      <c r="G67" s="46"/>
-      <c r="H67" s="46"/>
-      <c r="I67" s="46"/>
-      <c r="J67" s="46"/>
-      <c r="K67" s="84"/>
-      <c r="L67" s="46"/>
-      <c r="M67" s="46"/>
-      <c r="N67" s="84"/>
-      <c r="O67" s="46"/>
-      <c r="P67" s="67"/>
-      <c r="Q67" s="46"/>
-      <c r="R67" s="55">
+      <c r="D67" s="82"/>
+      <c r="E67" s="45"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="45"/>
+      <c r="H67" s="45"/>
+      <c r="I67" s="45"/>
+      <c r="J67" s="45"/>
+      <c r="K67" s="83"/>
+      <c r="L67" s="45"/>
+      <c r="M67" s="45"/>
+      <c r="N67" s="83"/>
+      <c r="O67" s="45"/>
+      <c r="P67" s="66"/>
+      <c r="Q67" s="45"/>
+      <c r="R67" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="2:18" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="154" t="s">
+      <c r="B68" s="153" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="83">
+      <c r="C68" s="82">
         <v>672</v>
       </c>
-      <c r="D68" s="46"/>
-      <c r="E68" s="46"/>
-      <c r="F68" s="46"/>
-      <c r="G68" s="46"/>
-      <c r="H68" s="46"/>
-      <c r="I68" s="46"/>
-      <c r="J68" s="46"/>
-      <c r="K68" s="84"/>
-      <c r="L68" s="46"/>
-      <c r="M68" s="46"/>
-      <c r="N68" s="84"/>
-      <c r="O68" s="46"/>
-      <c r="P68" s="67"/>
-      <c r="Q68" s="46"/>
-      <c r="R68" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:18" s="87" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="168" t="s">
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="45"/>
+      <c r="G68" s="45"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="45"/>
+      <c r="J68" s="45"/>
+      <c r="K68" s="83"/>
+      <c r="L68" s="45"/>
+      <c r="M68" s="45"/>
+      <c r="N68" s="83"/>
+      <c r="O68" s="45"/>
+      <c r="P68" s="66"/>
+      <c r="Q68" s="45"/>
+      <c r="R68" s="54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" s="86" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="154" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="168"/>
-      <c r="D69" s="168"/>
-      <c r="E69" s="168"/>
-      <c r="F69" s="168"/>
-      <c r="G69" s="168"/>
-      <c r="H69" s="168"/>
-      <c r="I69" s="168"/>
-      <c r="J69" s="168"/>
-      <c r="K69" s="168"/>
-      <c r="L69" s="168"/>
-      <c r="M69" s="168"/>
-      <c r="N69" s="169"/>
-      <c r="O69" s="168"/>
-      <c r="P69" s="168"/>
-      <c r="Q69" s="168"/>
-      <c r="R69" s="168"/>
+      <c r="C69" s="154"/>
+      <c r="D69" s="154"/>
+      <c r="E69" s="154"/>
+      <c r="F69" s="154"/>
+      <c r="G69" s="154"/>
+      <c r="H69" s="154"/>
+      <c r="I69" s="154"/>
+      <c r="J69" s="154"/>
+      <c r="K69" s="154"/>
+      <c r="L69" s="154"/>
+      <c r="M69" s="154"/>
+      <c r="N69" s="155"/>
+      <c r="O69" s="154"/>
+      <c r="P69" s="154"/>
+      <c r="Q69" s="154"/>
+      <c r="R69" s="154"/>
     </row>
     <row r="70" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="154" t="s">
+      <c r="B70" s="153" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="86">
+      <c r="C70" s="85">
         <v>28</v>
       </c>
-      <c r="D70" s="46"/>
-      <c r="E70" s="46"/>
-      <c r="F70" s="46"/>
-      <c r="G70" s="46"/>
-      <c r="H70" s="46"/>
-      <c r="I70" s="46"/>
-      <c r="J70" s="46"/>
-      <c r="K70" s="84"/>
-      <c r="L70" s="46"/>
-      <c r="M70" s="46"/>
-      <c r="N70" s="84"/>
-      <c r="O70" s="46"/>
-      <c r="P70" s="67"/>
-      <c r="Q70" s="46"/>
-      <c r="R70" s="55">
+      <c r="D70" s="45"/>
+      <c r="E70" s="45"/>
+      <c r="F70" s="45"/>
+      <c r="G70" s="45"/>
+      <c r="H70" s="45"/>
+      <c r="I70" s="45"/>
+      <c r="J70" s="45"/>
+      <c r="K70" s="83"/>
+      <c r="L70" s="45"/>
+      <c r="M70" s="45"/>
+      <c r="N70" s="83"/>
+      <c r="O70" s="45"/>
+      <c r="P70" s="66"/>
+      <c r="Q70" s="45"/>
+      <c r="R70" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="154" t="s">
+      <c r="B71" s="153" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="86">
+      <c r="C71" s="85">
         <v>28</v>
       </c>
-      <c r="D71" s="46"/>
-      <c r="E71" s="46"/>
-      <c r="F71" s="46"/>
-      <c r="G71" s="46"/>
-      <c r="H71" s="46"/>
-      <c r="I71" s="46"/>
-      <c r="J71" s="46"/>
-      <c r="K71" s="84"/>
-      <c r="L71" s="46"/>
-      <c r="M71" s="46"/>
-      <c r="N71" s="84"/>
-      <c r="O71" s="46"/>
-      <c r="P71" s="67"/>
-      <c r="Q71" s="46"/>
-      <c r="R71" s="55">
+      <c r="D71" s="45"/>
+      <c r="E71" s="45"/>
+      <c r="F71" s="45"/>
+      <c r="G71" s="45"/>
+      <c r="H71" s="45"/>
+      <c r="I71" s="45"/>
+      <c r="J71" s="45"/>
+      <c r="K71" s="83"/>
+      <c r="L71" s="45"/>
+      <c r="M71" s="45"/>
+      <c r="N71" s="83"/>
+      <c r="O71" s="45"/>
+      <c r="P71" s="66"/>
+      <c r="Q71" s="45"/>
+      <c r="R71" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="2:18" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B72" s="154" t="s">
+      <c r="B72" s="153" t="s">
         <v>64</v>
       </c>
-      <c r="C72" s="86">
+      <c r="C72" s="85">
         <v>30</v>
       </c>
-      <c r="D72" s="46"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="46"/>
-      <c r="H72" s="46"/>
-      <c r="I72" s="46"/>
-      <c r="J72" s="46"/>
-      <c r="K72" s="84"/>
-      <c r="L72" s="46"/>
-      <c r="M72" s="46"/>
-      <c r="N72" s="84"/>
-      <c r="O72" s="46"/>
-      <c r="P72" s="67"/>
-      <c r="Q72" s="46"/>
-      <c r="R72" s="55">
+      <c r="D72" s="45"/>
+      <c r="E72" s="45"/>
+      <c r="F72" s="45"/>
+      <c r="G72" s="45"/>
+      <c r="H72" s="45"/>
+      <c r="I72" s="45"/>
+      <c r="J72" s="45"/>
+      <c r="K72" s="83"/>
+      <c r="L72" s="45"/>
+      <c r="M72" s="45"/>
+      <c r="N72" s="83"/>
+      <c r="O72" s="45"/>
+      <c r="P72" s="66"/>
+      <c r="Q72" s="45"/>
+      <c r="R72" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="2:18" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="88"/>
-      <c r="C73" s="89"/>
+      <c r="B73" s="87"/>
+      <c r="C73" s="88"/>
     </row>
     <row r="74" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="P74" s="90"/>
-      <c r="Q74" s="90"/>
-      <c r="R74" s="90"/>
-    </row>
-    <row r="75" spans="2:18" s="94" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="91" t="s">
+      <c r="P74" s="89"/>
+      <c r="Q74" s="89"/>
+      <c r="R74" s="89"/>
+    </row>
+    <row r="75" spans="2:18" s="93" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="C75" s="90"/>
-      <c r="D75" s="92"/>
-      <c r="E75" s="92"/>
-      <c r="F75" s="92"/>
-      <c r="G75" s="92"/>
-      <c r="H75" s="92"/>
-      <c r="I75" s="92"/>
-      <c r="J75" s="92"/>
-      <c r="K75" s="92"/>
-      <c r="L75" s="92"/>
-      <c r="M75" s="92"/>
-      <c r="N75" s="92"/>
-      <c r="O75" s="92"/>
-      <c r="P75" s="92"/>
-      <c r="Q75" s="92"/>
-      <c r="R75" s="93"/>
-    </row>
-    <row r="76" spans="2:18" s="94" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="170"/>
-      <c r="C76" s="170"/>
-      <c r="D76" s="170"/>
-      <c r="E76" s="170"/>
-      <c r="F76" s="170"/>
-      <c r="G76" s="170"/>
-      <c r="H76" s="170"/>
-      <c r="I76" s="170"/>
-      <c r="J76" s="170"/>
-      <c r="K76" s="170"/>
-      <c r="L76" s="170"/>
-      <c r="M76" s="170"/>
-      <c r="N76" s="170"/>
-      <c r="O76" s="170"/>
-      <c r="P76" s="170"/>
-      <c r="Q76" s="170"/>
-      <c r="R76" s="170"/>
-    </row>
-    <row r="77" spans="2:18" s="94" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="171"/>
-      <c r="C77" s="171"/>
-      <c r="D77" s="171"/>
-      <c r="E77" s="171"/>
-      <c r="F77" s="171"/>
-      <c r="G77" s="171"/>
-      <c r="H77" s="171"/>
-      <c r="I77" s="171"/>
-      <c r="J77" s="171"/>
-      <c r="K77" s="171"/>
-      <c r="L77" s="171"/>
-      <c r="M77" s="171"/>
-      <c r="N77" s="171"/>
-      <c r="O77" s="171"/>
-      <c r="P77" s="171"/>
-      <c r="Q77" s="171"/>
-      <c r="R77" s="171"/>
-    </row>
-    <row r="78" spans="2:18" s="94" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="172"/>
-      <c r="C78" s="172"/>
-      <c r="D78" s="172"/>
-      <c r="E78" s="172"/>
-      <c r="F78" s="172"/>
-      <c r="G78" s="172"/>
-      <c r="H78" s="172"/>
-      <c r="I78" s="172"/>
-      <c r="J78" s="172"/>
-      <c r="K78" s="172"/>
-      <c r="L78" s="172"/>
-      <c r="M78" s="172"/>
-      <c r="N78" s="172"/>
-      <c r="O78" s="172"/>
-      <c r="P78" s="172"/>
-      <c r="Q78" s="172"/>
-      <c r="R78" s="172"/>
+      <c r="C75" s="89"/>
+      <c r="D75" s="91"/>
+      <c r="E75" s="91"/>
+      <c r="F75" s="91"/>
+      <c r="G75" s="91"/>
+      <c r="H75" s="91"/>
+      <c r="I75" s="91"/>
+      <c r="J75" s="91"/>
+      <c r="K75" s="91"/>
+      <c r="L75" s="91"/>
+      <c r="M75" s="91"/>
+      <c r="N75" s="91"/>
+      <c r="O75" s="91"/>
+      <c r="P75" s="91"/>
+      <c r="Q75" s="91"/>
+      <c r="R75" s="92"/>
+    </row>
+    <row r="76" spans="2:18" s="93" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="156"/>
+      <c r="C76" s="156"/>
+      <c r="D76" s="156"/>
+      <c r="E76" s="156"/>
+      <c r="F76" s="156"/>
+      <c r="G76" s="156"/>
+      <c r="H76" s="156"/>
+      <c r="I76" s="156"/>
+      <c r="J76" s="156"/>
+      <c r="K76" s="156"/>
+      <c r="L76" s="156"/>
+      <c r="M76" s="156"/>
+      <c r="N76" s="156"/>
+      <c r="O76" s="156"/>
+      <c r="P76" s="156"/>
+      <c r="Q76" s="156"/>
+      <c r="R76" s="156"/>
+    </row>
+    <row r="77" spans="2:18" s="93" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="157"/>
+      <c r="C77" s="157"/>
+      <c r="D77" s="157"/>
+      <c r="E77" s="157"/>
+      <c r="F77" s="157"/>
+      <c r="G77" s="157"/>
+      <c r="H77" s="157"/>
+      <c r="I77" s="157"/>
+      <c r="J77" s="157"/>
+      <c r="K77" s="157"/>
+      <c r="L77" s="157"/>
+      <c r="M77" s="157"/>
+      <c r="N77" s="157"/>
+      <c r="O77" s="157"/>
+      <c r="P77" s="157"/>
+      <c r="Q77" s="157"/>
+      <c r="R77" s="157"/>
+    </row>
+    <row r="78" spans="2:18" s="93" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="158"/>
+      <c r="C78" s="158"/>
+      <c r="D78" s="158"/>
+      <c r="E78" s="158"/>
+      <c r="F78" s="158"/>
+      <c r="G78" s="158"/>
+      <c r="H78" s="158"/>
+      <c r="I78" s="158"/>
+      <c r="J78" s="158"/>
+      <c r="K78" s="158"/>
+      <c r="L78" s="158"/>
+      <c r="M78" s="158"/>
+      <c r="N78" s="158"/>
+      <c r="O78" s="158"/>
+      <c r="P78" s="158"/>
+      <c r="Q78" s="158"/>
+      <c r="R78" s="158"/>
     </row>
     <row r="79" spans="2:18" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B79" s="95"/>
-      <c r="C79" s="96"/>
-    </row>
-    <row r="80" spans="2:18" s="12" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="95"/>
-      <c r="C80" s="96"/>
-      <c r="D80" s="90"/>
-      <c r="E80" s="90"/>
-      <c r="F80" s="90"/>
-      <c r="G80" s="90"/>
-      <c r="H80" s="90"/>
-      <c r="I80" s="90"/>
-      <c r="J80" s="90"/>
-      <c r="K80" s="90"/>
-      <c r="L80" s="90"/>
-      <c r="M80" s="90"/>
-      <c r="N80" s="90"/>
-      <c r="O80" s="90"/>
+      <c r="B79" s="94"/>
+      <c r="C79" s="95"/>
+    </row>
+    <row r="80" spans="2:18" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="94"/>
+      <c r="C80" s="95"/>
+      <c r="D80" s="89"/>
+      <c r="E80" s="89"/>
+      <c r="F80" s="89"/>
+      <c r="G80" s="89"/>
+      <c r="H80" s="89"/>
+      <c r="I80" s="89"/>
+      <c r="J80" s="89"/>
+      <c r="K80" s="89"/>
+      <c r="L80" s="89"/>
+      <c r="M80" s="89"/>
+      <c r="N80" s="89"/>
+      <c r="O80" s="89"/>
       <c r="P80" s="3"/>
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
     </row>
-    <row r="81" spans="2:21" s="12" customFormat="1" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:21" s="11" customFormat="1" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="1"/>
-      <c r="C81" s="90"/>
-      <c r="D81" s="90"/>
-      <c r="E81" s="90"/>
-      <c r="F81" s="90"/>
-      <c r="G81" s="90"/>
-      <c r="H81" s="90"/>
-      <c r="I81" s="90"/>
-      <c r="J81" s="90"/>
-      <c r="K81" s="90"/>
-      <c r="L81" s="90"/>
-      <c r="M81" s="90"/>
-      <c r="N81" s="90"/>
-      <c r="O81" s="90"/>
+      <c r="C81" s="89"/>
+      <c r="D81" s="89"/>
+      <c r="E81" s="89"/>
+      <c r="F81" s="89"/>
+      <c r="G81" s="89"/>
+      <c r="H81" s="89"/>
+      <c r="I81" s="89"/>
+      <c r="J81" s="89"/>
+      <c r="K81" s="89"/>
+      <c r="L81" s="89"/>
+      <c r="M81" s="89"/>
+      <c r="N81" s="89"/>
+      <c r="O81" s="89"/>
       <c r="P81" s="3"/>
       <c r="Q81" s="3"/>
       <c r="R81" s="3"/>
     </row>
-    <row r="82" spans="2:21" s="12" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="97" t="s">
+    <row r="82" spans="2:21" s="11" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="C82" s="98"/>
-      <c r="D82" s="99"/>
-      <c r="E82" s="100"/>
-      <c r="F82" s="100"/>
-      <c r="G82" s="100"/>
-      <c r="H82" s="100"/>
-      <c r="I82" s="100"/>
-      <c r="J82" s="100"/>
-      <c r="K82" s="100"/>
-      <c r="L82" s="100"/>
-      <c r="M82" s="100"/>
-      <c r="N82" s="100"/>
-      <c r="O82" s="100"/>
-      <c r="P82" s="100"/>
-      <c r="Q82" s="100"/>
-      <c r="R82" s="100"/>
-    </row>
-    <row r="83" spans="2:21" s="12" customFormat="1" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="B83" s="101"/>
-      <c r="C83" s="102" t="s">
+      <c r="C82" s="97"/>
+      <c r="D82" s="98"/>
+      <c r="E82" s="99"/>
+      <c r="F82" s="99"/>
+      <c r="G82" s="99"/>
+      <c r="H82" s="99"/>
+      <c r="I82" s="99"/>
+      <c r="J82" s="99"/>
+      <c r="K82" s="99"/>
+      <c r="L82" s="99"/>
+      <c r="M82" s="99"/>
+      <c r="N82" s="99"/>
+      <c r="O82" s="99"/>
+      <c r="P82" s="99"/>
+      <c r="Q82" s="99"/>
+      <c r="R82" s="99"/>
+    </row>
+    <row r="83" spans="2:21" s="11" customFormat="1" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="B83" s="100"/>
+      <c r="C83" s="101" t="s">
         <v>67</v>
       </c>
-      <c r="D83" s="103"/>
-      <c r="E83" s="103"/>
-      <c r="F83" s="103"/>
-      <c r="G83" s="9"/>
-      <c r="I83" s="9"/>
-      <c r="J83" s="102" t="s">
+      <c r="D83" s="102"/>
+      <c r="E83" s="102"/>
+      <c r="F83" s="102"/>
+      <c r="G83" s="8"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="K83" s="9"/>
-      <c r="L83" s="103"/>
-      <c r="M83" s="103"/>
-      <c r="N83" s="9"/>
-      <c r="O83" s="9"/>
-    </row>
-    <row r="84" spans="2:21" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="104"/>
-      <c r="C84" s="105" t="s">
+      <c r="K83" s="8"/>
+      <c r="L83" s="102"/>
+      <c r="M83" s="102"/>
+      <c r="N83" s="8"/>
+      <c r="O83" s="8"/>
+    </row>
+    <row r="84" spans="2:21" s="11" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="103"/>
+      <c r="C84" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="9"/>
-      <c r="J84" s="9"/>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
-      <c r="M84" s="9"/>
-      <c r="N84" s="9"/>
-      <c r="O84" s="9"/>
-    </row>
-    <row r="85" spans="2:21" s="106" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="17"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
-      <c r="H85" s="9"/>
-      <c r="I85" s="9"/>
-      <c r="J85" s="9"/>
-      <c r="K85" s="9"/>
-      <c r="L85" s="9"/>
-      <c r="M85" s="9"/>
-      <c r="N85" s="9"/>
-      <c r="O85" s="9"/>
-      <c r="P85" s="12"/>
-      <c r="Q85" s="12"/>
-      <c r="R85" s="12"/>
-    </row>
-    <row r="86" spans="2:21" s="77" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="97" t="s">
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="8"/>
+      <c r="N84" s="8"/>
+      <c r="O84" s="8"/>
+    </row>
+    <row r="85" spans="2:21" s="105" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B85" s="16"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="8"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="8"/>
+      <c r="O85" s="8"/>
+      <c r="P85" s="11"/>
+      <c r="Q85" s="11"/>
+      <c r="R85" s="11"/>
+    </row>
+    <row r="86" spans="2:21" s="76" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="C86" s="98"/>
-      <c r="D86" s="99"/>
-      <c r="E86" s="100"/>
-      <c r="F86" s="100"/>
-      <c r="G86" s="100"/>
-      <c r="H86" s="100"/>
-      <c r="I86" s="100"/>
-      <c r="J86" s="100"/>
-      <c r="K86" s="100"/>
-      <c r="L86" s="100"/>
-      <c r="M86" s="100"/>
-      <c r="N86" s="100"/>
-      <c r="O86" s="100"/>
-      <c r="P86" s="100"/>
-      <c r="Q86" s="100"/>
-      <c r="R86" s="100"/>
-      <c r="S86" s="76"/>
-      <c r="T86" s="76"/>
-      <c r="U86" s="76"/>
+      <c r="C86" s="97"/>
+      <c r="D86" s="98"/>
+      <c r="E86" s="99"/>
+      <c r="F86" s="99"/>
+      <c r="G86" s="99"/>
+      <c r="H86" s="99"/>
+      <c r="I86" s="99"/>
+      <c r="J86" s="99"/>
+      <c r="K86" s="99"/>
+      <c r="L86" s="99"/>
+      <c r="M86" s="99"/>
+      <c r="N86" s="99"/>
+      <c r="O86" s="99"/>
+      <c r="P86" s="99"/>
+      <c r="Q86" s="99"/>
+      <c r="R86" s="99"/>
+      <c r="S86" s="75"/>
+      <c r="T86" s="75"/>
+      <c r="U86" s="75"/>
     </row>
     <row r="87" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="107" t="s">
+      <c r="B87" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="C87" s="108"/>
-      <c r="D87" s="109"/>
-      <c r="E87" s="110"/>
-      <c r="F87" s="110"/>
-      <c r="G87" s="110"/>
-      <c r="H87" s="110"/>
-      <c r="I87" s="110"/>
-      <c r="J87" s="110"/>
-      <c r="K87" s="110"/>
-      <c r="L87" s="110"/>
-      <c r="M87" s="110"/>
-      <c r="N87" s="110"/>
-      <c r="O87" s="110"/>
-      <c r="P87" s="110"/>
-      <c r="Q87" s="110"/>
-      <c r="R87" s="110"/>
+      <c r="C87" s="107"/>
+      <c r="D87" s="108"/>
+      <c r="E87" s="109"/>
+      <c r="F87" s="109"/>
+      <c r="G87" s="109"/>
+      <c r="H87" s="109"/>
+      <c r="I87" s="109"/>
+      <c r="J87" s="109"/>
+      <c r="K87" s="109"/>
+      <c r="L87" s="109"/>
+      <c r="M87" s="109"/>
+      <c r="N87" s="109"/>
+      <c r="O87" s="109"/>
+      <c r="P87" s="109"/>
+      <c r="Q87" s="109"/>
+      <c r="R87" s="109"/>
       <c r="T87" s="4"/>
       <c r="U87" s="4"/>
     </row>
     <row r="88" spans="2:21" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="111"/>
-      <c r="C88" s="112"/>
-      <c r="D88" s="113"/>
-      <c r="E88" s="114"/>
-      <c r="F88" s="114"/>
-      <c r="G88" s="114"/>
-      <c r="H88" s="114"/>
-      <c r="I88" s="114"/>
-      <c r="J88" s="114"/>
-      <c r="K88" s="114"/>
-      <c r="L88" s="114"/>
-      <c r="M88" s="114"/>
-      <c r="N88" s="114"/>
-      <c r="O88" s="114"/>
-      <c r="P88" s="114"/>
-      <c r="Q88" s="114"/>
-      <c r="R88" s="114"/>
+      <c r="B88" s="110"/>
+      <c r="C88" s="111"/>
+      <c r="D88" s="112"/>
+      <c r="E88" s="113"/>
+      <c r="F88" s="113"/>
+      <c r="G88" s="113"/>
+      <c r="H88" s="113"/>
+      <c r="I88" s="113"/>
+      <c r="J88" s="113"/>
+      <c r="K88" s="113"/>
+      <c r="L88" s="113"/>
+      <c r="M88" s="113"/>
+      <c r="N88" s="113"/>
+      <c r="O88" s="113"/>
+      <c r="P88" s="113"/>
+      <c r="Q88" s="113"/>
+      <c r="R88" s="113"/>
       <c r="T88" s="4"/>
       <c r="U88" s="4"/>
     </row>
     <row r="89" spans="2:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="112"/>
-      <c r="C89" s="112"/>
-      <c r="D89" s="115" t="s">
+      <c r="B89" s="111"/>
+      <c r="C89" s="111"/>
+      <c r="D89" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="E89" s="116" t="s">
+      <c r="E89" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="F89" s="117"/>
-      <c r="G89" s="118" t="s">
+      <c r="F89" s="116"/>
+      <c r="G89" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="H89" s="118" t="s">
+      <c r="H89" s="117" t="s">
         <v>75</v>
       </c>
-      <c r="I89" s="118" t="s">
+      <c r="I89" s="117" t="s">
         <v>76</v>
       </c>
-      <c r="J89" s="119" t="s">
+      <c r="J89" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="K89" s="120"/>
-      <c r="L89" s="120"/>
-      <c r="M89" s="120"/>
-      <c r="N89" s="120"/>
-      <c r="P89" s="114"/>
+      <c r="K89" s="119"/>
+      <c r="L89" s="119"/>
+      <c r="M89" s="119"/>
+      <c r="N89" s="119"/>
+      <c r="P89" s="113"/>
       <c r="T89" s="4"/>
       <c r="U89" s="4"/>
     </row>
     <row r="90" spans="2:21" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="112"/>
-      <c r="C90" s="112"/>
-      <c r="D90" s="121" t="s">
+      <c r="B90" s="111"/>
+      <c r="C90" s="111"/>
+      <c r="D90" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="E90" s="116" t="s">
+      <c r="E90" s="115" t="s">
         <v>79</v>
       </c>
-      <c r="F90" s="122"/>
-      <c r="G90" s="123"/>
-      <c r="H90" s="124"/>
-      <c r="I90" s="123"/>
-      <c r="J90" s="125"/>
-      <c r="K90" s="126"/>
-      <c r="L90" s="126"/>
-      <c r="M90" s="126"/>
-      <c r="N90" s="126"/>
-      <c r="P90" s="114"/>
+      <c r="F90" s="121"/>
+      <c r="G90" s="122"/>
+      <c r="H90" s="123"/>
+      <c r="I90" s="122"/>
+      <c r="J90" s="124"/>
+      <c r="K90" s="125"/>
+      <c r="L90" s="125"/>
+      <c r="M90" s="125"/>
+      <c r="N90" s="125"/>
+      <c r="P90" s="113"/>
       <c r="T90" s="4"/>
       <c r="U90" s="4"/>
     </row>
     <row r="91" spans="2:21" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="112"/>
-      <c r="C91" s="112"/>
-      <c r="D91" s="127" t="s">
+      <c r="B91" s="111"/>
+      <c r="C91" s="111"/>
+      <c r="D91" s="126" t="s">
         <v>80</v>
       </c>
-      <c r="E91" s="128" t="s">
+      <c r="E91" s="127" t="s">
         <v>81</v>
       </c>
-      <c r="F91" s="129" t="s">
+      <c r="F91" s="128" t="s">
         <v>82</v>
       </c>
-      <c r="G91" s="130"/>
-      <c r="H91" s="131"/>
-      <c r="I91" s="130"/>
-      <c r="J91" s="132"/>
-      <c r="K91" s="126"/>
-      <c r="L91" s="126"/>
-      <c r="M91" s="126"/>
-      <c r="N91" s="126"/>
-      <c r="P91" s="114"/>
+      <c r="G91" s="129"/>
+      <c r="H91" s="130"/>
+      <c r="I91" s="129"/>
+      <c r="J91" s="131"/>
+      <c r="K91" s="125"/>
+      <c r="L91" s="125"/>
+      <c r="M91" s="125"/>
+      <c r="N91" s="125"/>
+      <c r="P91" s="113"/>
     </row>
     <row r="92" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="112"/>
-      <c r="C92" s="112"/>
-      <c r="D92" s="133" t="s">
+      <c r="B92" s="111"/>
+      <c r="C92" s="111"/>
+      <c r="D92" s="132" t="s">
         <v>83</v>
       </c>
-      <c r="E92" s="134"/>
-      <c r="F92" s="135"/>
-      <c r="G92" s="136"/>
-      <c r="H92" s="136"/>
-      <c r="I92" s="136"/>
-      <c r="J92" s="137"/>
-      <c r="K92" s="138"/>
-      <c r="L92" s="138"/>
-      <c r="M92" s="138"/>
-      <c r="N92" s="138"/>
-      <c r="P92" s="114"/>
+      <c r="E92" s="133"/>
+      <c r="F92" s="134"/>
+      <c r="G92" s="135"/>
+      <c r="H92" s="135"/>
+      <c r="I92" s="135"/>
+      <c r="J92" s="136"/>
+      <c r="K92" s="137"/>
+      <c r="L92" s="137"/>
+      <c r="M92" s="137"/>
+      <c r="N92" s="137"/>
+      <c r="P92" s="113"/>
     </row>
     <row r="93" spans="2:21" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="112"/>
-      <c r="C93" s="112"/>
-      <c r="D93" s="113"/>
-      <c r="E93" s="114"/>
-      <c r="F93" s="114"/>
-      <c r="G93" s="114"/>
-      <c r="H93" s="114"/>
-      <c r="I93" s="139"/>
-      <c r="J93" s="114"/>
-      <c r="K93" s="114"/>
-      <c r="L93" s="114"/>
-      <c r="M93" s="114"/>
-      <c r="N93" s="114"/>
+      <c r="B93" s="111"/>
+      <c r="C93" s="111"/>
+      <c r="D93" s="112"/>
+      <c r="E93" s="113"/>
+      <c r="F93" s="113"/>
+      <c r="G93" s="113"/>
+      <c r="H93" s="113"/>
+      <c r="I93" s="138"/>
+      <c r="J93" s="113"/>
+      <c r="K93" s="113"/>
+      <c r="L93" s="113"/>
+      <c r="M93" s="113"/>
+      <c r="N93" s="113"/>
       <c r="P93" s="4"/>
-      <c r="Q93" s="114"/>
-      <c r="R93" s="114"/>
+      <c r="Q93" s="113"/>
+      <c r="R93" s="113"/>
     </row>
     <row r="94" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B94" s="112"/>
-      <c r="C94" s="112"/>
-      <c r="D94" s="113"/>
-      <c r="E94" s="114"/>
-      <c r="F94" s="114"/>
-      <c r="G94" s="114"/>
-      <c r="H94" s="114"/>
-      <c r="I94" s="114"/>
-      <c r="J94" s="114"/>
-      <c r="K94" s="114"/>
-      <c r="L94" s="114"/>
-      <c r="M94" s="114"/>
-      <c r="N94" s="114"/>
-      <c r="O94" s="114"/>
-      <c r="P94" s="114"/>
-      <c r="Q94" s="114"/>
-      <c r="R94" s="114"/>
+      <c r="B94" s="111"/>
+      <c r="C94" s="111"/>
+      <c r="D94" s="112"/>
+      <c r="E94" s="113"/>
+      <c r="F94" s="113"/>
+      <c r="G94" s="113"/>
+      <c r="H94" s="113"/>
+      <c r="I94" s="113"/>
+      <c r="J94" s="113"/>
+      <c r="K94" s="113"/>
+      <c r="L94" s="113"/>
+      <c r="M94" s="113"/>
+      <c r="N94" s="113"/>
+      <c r="O94" s="113"/>
+      <c r="P94" s="113"/>
+      <c r="Q94" s="113"/>
+      <c r="R94" s="113"/>
     </row>
     <row r="95" spans="2:21" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B95" s="140" t="s">
+      <c r="B95" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="C95" s="92"/>
-      <c r="D95" s="92"/>
-      <c r="E95" s="92"/>
-      <c r="F95" s="141"/>
-      <c r="G95" s="140" t="s">
+      <c r="C95" s="91"/>
+      <c r="D95" s="91"/>
+      <c r="E95" s="91"/>
+      <c r="F95" s="140"/>
+      <c r="G95" s="139" t="s">
         <v>85</v>
       </c>
-      <c r="H95" s="92"/>
-      <c r="I95" s="92"/>
-      <c r="J95" s="92"/>
-      <c r="K95" s="142"/>
-      <c r="L95" s="142"/>
-      <c r="M95" s="140" t="s">
+      <c r="H95" s="91"/>
+      <c r="I95" s="91"/>
+      <c r="J95" s="91"/>
+      <c r="K95" s="141"/>
+      <c r="L95" s="141"/>
+      <c r="M95" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="N95" s="92"/>
-      <c r="O95" s="92"/>
-      <c r="P95" s="92"/>
-      <c r="Q95" s="92"/>
-      <c r="R95" s="92"/>
+      <c r="N95" s="91"/>
+      <c r="O95" s="91"/>
+      <c r="P95" s="91"/>
+      <c r="Q95" s="91"/>
+      <c r="R95" s="91"/>
     </row>
     <row r="96" spans="2:21" ht="21" x14ac:dyDescent="0.4">
-      <c r="B96" s="143"/>
-      <c r="D96" s="143" t="s">
+      <c r="B96" s="142"/>
+      <c r="D96" s="142" t="s">
         <v>87</v>
       </c>
-      <c r="F96" s="144"/>
-      <c r="G96" s="145"/>
-      <c r="O96" s="144"/>
-      <c r="P96" s="146"/>
+      <c r="F96" s="143"/>
+      <c r="G96" s="144"/>
+      <c r="O96" s="143"/>
+      <c r="P96" s="145"/>
     </row>
     <row r="97" spans="2:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B97" s="140" t="s">
+      <c r="B97" s="139" t="s">
         <v>88</v>
       </c>
-      <c r="C97" s="92"/>
-      <c r="D97" s="92"/>
-      <c r="E97" s="92"/>
-      <c r="F97" s="147"/>
-      <c r="G97" s="140" t="s">
+      <c r="C97" s="91"/>
+      <c r="D97" s="91"/>
+      <c r="E97" s="91"/>
+      <c r="F97" s="146"/>
+      <c r="G97" s="139" t="s">
         <v>89</v>
       </c>
-      <c r="H97" s="92"/>
-      <c r="I97" s="92"/>
-      <c r="J97" s="92"/>
-      <c r="K97" s="142"/>
-      <c r="L97" s="142"/>
-      <c r="M97" s="142"/>
-      <c r="N97" s="142"/>
-      <c r="P97" s="146"/>
+      <c r="H97" s="91"/>
+      <c r="I97" s="91"/>
+      <c r="J97" s="91"/>
+      <c r="K97" s="141"/>
+      <c r="L97" s="141"/>
+      <c r="M97" s="141"/>
+      <c r="N97" s="141"/>
+      <c r="P97" s="145"/>
     </row>
     <row r="98" spans="2:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B98" s="148"/>
-      <c r="F98" s="141"/>
-      <c r="G98" s="145"/>
-      <c r="P98" s="146"/>
+      <c r="B98" s="147"/>
+      <c r="F98" s="140"/>
+      <c r="G98" s="144"/>
+      <c r="P98" s="145"/>
     </row>
     <row r="99" spans="2:18" ht="21" x14ac:dyDescent="0.4">
-      <c r="B99" s="148"/>
-      <c r="F99" s="141"/>
-      <c r="G99" s="145"/>
-      <c r="P99" s="146"/>
+      <c r="B99" s="147"/>
+      <c r="F99" s="140"/>
+      <c r="G99" s="144"/>
+      <c r="P99" s="145"/>
     </row>
     <row r="100" spans="2:18" ht="28.2" x14ac:dyDescent="0.5">
-      <c r="B100" s="140" t="s">
+      <c r="B100" s="139" t="s">
         <v>90</v>
       </c>
-      <c r="C100" s="92"/>
-      <c r="D100" s="92"/>
-      <c r="E100" s="92"/>
-      <c r="F100" s="141"/>
-      <c r="G100" s="140" t="s">
+      <c r="C100" s="91"/>
+      <c r="D100" s="91"/>
+      <c r="E100" s="91"/>
+      <c r="F100" s="140"/>
+      <c r="G100" s="139" t="s">
         <v>85</v>
       </c>
-      <c r="H100" s="92"/>
-      <c r="I100" s="92"/>
-      <c r="J100" s="92"/>
-      <c r="K100" s="142"/>
-      <c r="L100" s="142"/>
-      <c r="M100" s="140" t="s">
+      <c r="H100" s="91"/>
+      <c r="I100" s="91"/>
+      <c r="J100" s="91"/>
+      <c r="K100" s="141"/>
+      <c r="L100" s="141"/>
+      <c r="M100" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="N100" s="92"/>
-      <c r="O100" s="92"/>
-      <c r="P100" s="92"/>
-      <c r="Q100" s="92"/>
-      <c r="R100" s="92"/>
+      <c r="N100" s="91"/>
+      <c r="O100" s="91"/>
+      <c r="P100" s="91"/>
+      <c r="Q100" s="91"/>
+      <c r="R100" s="91"/>
     </row>
     <row r="101" spans="2:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B101" s="143"/>
-      <c r="D101" s="143" t="s">
+      <c r="B101" s="142"/>
+      <c r="D101" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="F101" s="144"/>
-      <c r="G101" s="145"/>
-      <c r="O101" s="144"/>
-      <c r="P101" s="149"/>
+      <c r="F101" s="143"/>
+      <c r="G101" s="144"/>
+      <c r="O101" s="143"/>
+      <c r="P101" s="148"/>
     </row>
     <row r="102" spans="2:18" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B102" s="148"/>
-      <c r="F102" s="141"/>
-      <c r="G102" s="150"/>
+      <c r="B102" s="147"/>
+      <c r="F102" s="140"/>
+      <c r="G102" s="149"/>
     </row>
     <row r="103" spans="2:18" ht="28.2" x14ac:dyDescent="0.5">
-      <c r="B103" s="140" t="s">
+      <c r="B103" s="139" t="s">
         <v>88</v>
       </c>
-      <c r="C103" s="92"/>
-      <c r="D103" s="92"/>
-      <c r="E103" s="92"/>
-      <c r="F103" s="147"/>
-      <c r="G103" s="140" t="s">
+      <c r="C103" s="91"/>
+      <c r="D103" s="91"/>
+      <c r="E103" s="91"/>
+      <c r="F103" s="146"/>
+      <c r="G103" s="139" t="s">
         <v>89</v>
       </c>
-      <c r="H103" s="92"/>
-      <c r="I103" s="92"/>
-      <c r="J103" s="92"/>
-      <c r="K103" s="142"/>
-      <c r="L103" s="142"/>
-      <c r="M103" s="142"/>
-      <c r="N103" s="142"/>
+      <c r="H103" s="91"/>
+      <c r="I103" s="91"/>
+      <c r="J103" s="91"/>
+      <c r="K103" s="141"/>
+      <c r="L103" s="141"/>
+      <c r="M103" s="141"/>
+      <c r="N103" s="141"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B69:N69"/>
-    <mergeCell ref="O69:R69"/>
-    <mergeCell ref="B76:R78"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B15:R15"/>
+  <mergeCells count="20">
+    <mergeCell ref="B2:Q2"/>
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="O10:R10"/>
@@ -4750,6 +4743,15 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="B69:N69"/>
+    <mergeCell ref="O69:R69"/>
+    <mergeCell ref="B76:R78"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B15:R15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>